<commit_message>
Adding missing files from previous commit
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/WebinarData.xlsx
+++ b/ProvarProject/templates/WebinarData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\ProvarIntegrations\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1CEFB2-A3F2-4878-A494-F5F6B14E4371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E1FDBF-430C-4257-AB90-A669E52E3828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{B349D999-C093-3947-8F7D-78D74E4E76F2}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="24420" windowHeight="15720" activeTab="2" xr2:uid="{B349D999-C093-3947-8F7D-78D74E4E76F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId1"/>
     <sheet name="Leads" sheetId="3" r:id="rId2"/>
-    <sheet name="Opportunities" sheetId="2" r:id="rId3"/>
+    <sheet name="Properties" sheetId="4" r:id="rId3"/>
+    <sheet name="Opportunities" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Active</t>
   </si>
@@ -107,6 +108,33 @@
   </si>
   <si>
     <t>Web</t>
+  </si>
+  <si>
+    <t>AskingPrice</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Baths</t>
+  </si>
+  <si>
+    <t>Cambridge</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Broker</t>
+  </si>
+  <si>
+    <t>Victor Ochoa</t>
   </si>
 </sst>
 </file>
@@ -151,10 +179,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122070D-9106-4FC1-B7DB-5A048C0E80DA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -602,6 +632,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195DFC35-19F9-472F-AEAB-7937535CAB8E}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="20.5625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.3125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.4375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>450000</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF44DB7-8F54-46F3-B7B6-FAAA6C738CF9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -637,7 +730,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">TODAY()+7</f>
-        <v>43858</v>
+        <v>44098</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>

</xml_diff>